<commit_message>
THR Tools Update with X4 DMR format
</commit_message>
<xml_diff>
--- a/PPV/parsers/MCChecker/CWF/##Name##_##w##_##LABEL##_PPV_Unit_Overview.xlsx
+++ b/PPV/parsers/MCChecker/CWF/##Name##_##w##_##LABEL##_PPV_Unit_Overview.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\Automation\PPV\MCChecker\CWF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\PPV\parsers\MCChecker\CWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD021F9C-EA73-4B6D-81C9-F0D7124A8A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155A66EF-6F2E-40F8-97FF-3FEFF0066208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B533D783-8E94-47EE-A5E0-31DB8C66C10E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B533D783-8E94-47EE-A5E0-31DB8C66C10E}"/>
   </bookViews>
   <sheets>
     <sheet name="CHA" sheetId="1" r:id="rId1"/>
     <sheet name="CORE" sheetId="5" r:id="rId2"/>
     <sheet name="PPV" sheetId="3" r:id="rId3"/>
     <sheet name="MC_Check" sheetId="2" r:id="rId4"/>
-    <sheet name="ErrorData" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="ErrorData" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="splitchar" comment="Change if using pysv registers or dpmb format">ErrorData!$G$1</definedName>
@@ -3155,21 +3155,21 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="105.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1"/>
-    <col min="10" max="10" width="105.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="105.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" customWidth="1"/>
+    <col min="10" max="10" width="105.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -3303,7 +3303,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -3385,21 +3385,21 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="105.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1"/>
-    <col min="10" max="10" width="105.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="105.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" customWidth="1"/>
+    <col min="10" max="10" width="105.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -3550,29 +3550,29 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="13.44140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="5.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="8.109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="7.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="86.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5546875" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" customWidth="1"/>
-    <col min="13" max="15" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" customWidth="1"/>
+    <col min="4" max="4" width="5.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="13.453125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="5.90625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="7.54296875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="86.1796875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.54296875" customWidth="1"/>
+    <col min="12" max="12" width="26.6328125" customWidth="1"/>
+    <col min="13" max="15" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="44" t="s">
         <v>2</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B5" s="47" t="s">
         <v>35</v>
       </c>
@@ -3644,44 +3644,44 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AM59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AL6" sqref="AL6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.109375" customWidth="1"/>
-    <col min="4" max="4" width="46.88671875" customWidth="1"/>
-    <col min="5" max="5" width="33.77734375" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
-    <col min="9" max="9" width="2.88671875" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.08984375" customWidth="1"/>
+    <col min="4" max="4" width="46.90625" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="6" max="6" width="5.36328125" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="2.90625" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.6640625" customWidth="1"/>
-    <col min="24" max="24" width="6.77734375" customWidth="1"/>
-    <col min="25" max="25" width="0.5546875" customWidth="1"/>
-    <col min="26" max="26" width="6.77734375" customWidth="1"/>
-    <col min="27" max="27" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="0.5546875" customWidth="1"/>
-    <col min="29" max="29" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.6640625" customWidth="1"/>
-    <col min="32" max="32" width="0.5546875" customWidth="1"/>
-    <col min="33" max="33" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="0.5546875" customWidth="1"/>
-    <col min="36" max="36" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="8.88671875" customWidth="1"/>
+    <col min="13" max="22" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.6328125" customWidth="1"/>
+    <col min="24" max="24" width="6.81640625" customWidth="1"/>
+    <col min="25" max="25" width="0.54296875" customWidth="1"/>
+    <col min="26" max="26" width="6.81640625" customWidth="1"/>
+    <col min="27" max="27" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="0.54296875" customWidth="1"/>
+    <col min="29" max="29" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.6328125" customWidth="1"/>
+    <col min="32" max="32" width="0.54296875" customWidth="1"/>
+    <col min="33" max="33" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="0.54296875" customWidth="1"/>
+    <col min="36" max="36" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="86"/>
       <c r="B1" s="50" t="s">
         <v>89</v>
@@ -3731,7 +3731,7 @@
       <c r="AL1" s="86"/>
       <c r="AM1" s="86"/>
     </row>
-    <row r="2" spans="1:39" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="86"/>
       <c r="B2" s="8" t="s">
         <v>20</v>
@@ -3797,7 +3797,7 @@
       <c r="AL2" s="86"/>
       <c r="AM2" s="86"/>
     </row>
-    <row r="3" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="86"/>
       <c r="B3" s="1" t="str" cm="1">
         <f t="array" ref="B3">IF(C1="All",_xlfn.UNIQUE(ppv[VisualId]),_xlfn._xlws.FILTER(ppv[VisualId],(ppv[SubBucket]=C1)*(IF(D1&lt;&gt;"",ISNUMBER(SEARCH(D1, ppv[Comments])),TRUE))))</f>
@@ -3882,7 +3882,7 @@
       <c r="AL3" s="86"/>
       <c r="AM3" s="86"/>
     </row>
-    <row r="4" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="86"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="str">
@@ -3974,7 +3974,7 @@
       <c r="AL4" s="86"/>
       <c r="AM4" s="86"/>
     </row>
-    <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="86"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="str">
@@ -4049,39 +4049,39 @@
       </c>
       <c r="AB5" s="74"/>
       <c r="AC5" s="81" t="str" cm="1">
-        <f t="array" ref="AC5">IFERROR("PHY"&amp;_xlfn._xlws.FILTER(misc[location],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-$AG$2,1)),"")&amp;":"&amp;IFERROR("MODULE"&amp;_xlfn._xlws.FILTER(misc[Module],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AC5">IFERROR("PHY"&amp;_xlfn._xlws.FILTER(misc[location],misc[Core_Hitter_Count]&gt;MAX(misc[Core_Hitter_Count]-$AG$2,0)),"")&amp;":"&amp;IFERROR("MODULE"&amp;_xlfn._xlws.FILTER(misc[Module],misc[Core_Hitter_Count]&gt;MAX(misc[Core_Hitter_Count]-$AG$2,)),"")</f>
         <v>:</v>
       </c>
       <c r="AD5" s="78" t="str" cm="1">
-        <f t="array" ref="AD5">IFERROR(_xlfn._xlws.FILTER(misc[Core_Hitter_Count],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AD5">IFERROR(_xlfn._xlws.FILTER(misc[Core_Hitter_Count],misc[Core_Hitter_Count]&gt;MAX(misc[Core_Hitter_Count]-$AG$2,0)),"")</f>
         <v/>
       </c>
       <c r="AE5" s="88" t="str" cm="1">
-        <f t="array" ref="AE5">IFERROR(_xlfn._xlws.FILTER(misc[Core_FAILS],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AE5">IFERROR(_xlfn._xlws.FILTER(misc[Core_FAILS],misc[Core_Hitter_Count]&gt;MAX(misc[Core_Hitter_Count]-$AG$2,0)),"")</f>
         <v/>
       </c>
       <c r="AF5" s="68"/>
       <c r="AG5" s="87" t="str" cm="1">
-        <f t="array" ref="AG5">IFERROR("CHA"&amp;_xlfn._xlws.FILTER(misc[location],misc[CHA_Hitter_Count]&gt;=MAX(misc[CHA_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AG5">IFERROR("CHA"&amp;_xlfn._xlws.FILTER(misc[location],misc[CHA_Hitter_Count]&gt;MAX(misc[CHA_Hitter_Count]-$AG$2,0)),"")</f>
         <v/>
       </c>
       <c r="AH5" s="78" t="str" cm="1">
-        <f t="array" ref="AH5">IFERROR(_xlfn._xlws.FILTER(misc[CHA_Hitter_Count],misc[CHA_Hitter_Count]&gt;=MAX(misc[CHA_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AH5">IFERROR(_xlfn._xlws.FILTER(misc[CHA_Hitter_Count],misc[CHA_Hitter_Count]&gt;MAX(misc[CHA_Hitter_Count]-$AG$2,0)),"")</f>
         <v/>
       </c>
       <c r="AI5" s="68"/>
       <c r="AJ5" s="87" t="str" cm="1">
-        <f t="array" ref="AJ5">IFERROR("LLC"&amp;_xlfn._xlws.FILTER(misc[location],misc[LLC_Hitter_Count]&gt;=MAX(misc[LLC_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AJ5">IFERROR("LLC"&amp;_xlfn._xlws.FILTER(misc[location],misc[LLC_Hitter_Count]&gt;MAX(misc[LLC_Hitter_Count]-$AG$2,0)),"")</f>
         <v/>
       </c>
       <c r="AK5" s="78" t="str" cm="1">
-        <f t="array" ref="AK5">IFERROR(_xlfn._xlws.FILTER(misc[LLC_Hitter_Count],misc[LLC_Hitter_Count]&gt;=MAX(misc[LLC_Hitter_Count]-$AG$2,1)),"")</f>
+        <f t="array" ref="AK5">IFERROR(_xlfn._xlws.FILTER(misc[LLC_Hitter_Count],misc[LLC_Hitter_Count]&gt;MAX(misc[LLC_Hitter_Count]-$AG$2,0)),"")</f>
         <v/>
       </c>
       <c r="AL5" s="86"/>
       <c r="AM5" s="86"/>
     </row>
-    <row r="6" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="86"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="str">
@@ -4158,7 +4158,7 @@
       <c r="AL6" s="86"/>
       <c r="AM6" s="86"/>
     </row>
-    <row r="7" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="86"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="str">
@@ -4233,7 +4233,7 @@
       <c r="AL7" s="86"/>
       <c r="AM7" s="86"/>
     </row>
-    <row r="8" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="86"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="str">
@@ -4312,7 +4312,7 @@
       <c r="AL8" s="86"/>
       <c r="AM8" s="86"/>
     </row>
-    <row r="9" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="86"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="str">
@@ -4385,7 +4385,7 @@
       <c r="AL9" s="86"/>
       <c r="AM9" s="86"/>
     </row>
-    <row r="10" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="86"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="str">
@@ -4458,7 +4458,7 @@
       <c r="AL10" s="86"/>
       <c r="AM10" s="86"/>
     </row>
-    <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="86"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="str">
@@ -4533,7 +4533,7 @@
       <c r="AL11" s="86"/>
       <c r="AM11" s="86"/>
     </row>
-    <row r="12" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="86"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="str">
@@ -4579,7 +4579,10 @@
       <c r="V12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="X12" s="79"/>
+      <c r="X12" s="79" t="str" cm="1">
+        <f t="array" ref="X12">IFERROR(_xlfn._xlws.FILTER(s3errors[type],s3errors[Counter]&gt;0),"")</f>
+        <v/>
+      </c>
       <c r="Y12" s="74"/>
       <c r="Z12" s="84"/>
       <c r="AA12" s="76"/>
@@ -4596,7 +4599,7 @@
       <c r="AL12" s="86"/>
       <c r="AM12" s="86"/>
     </row>
-    <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="86"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="str">
@@ -4626,7 +4629,7 @@
       <c r="AL13" s="86"/>
       <c r="AM13" s="86"/>
     </row>
-    <row r="14" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="86"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="str">
@@ -4692,7 +4695,7 @@
       <c r="AL14" s="86"/>
       <c r="AM14" s="86"/>
     </row>
-    <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="86"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="str">
@@ -4758,7 +4761,7 @@
       <c r="AL15" s="86"/>
       <c r="AM15" s="86"/>
     </row>
-    <row r="16" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="86"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="str">
@@ -4831,7 +4834,7 @@
       <c r="AL16" s="86"/>
       <c r="AM16" s="86"/>
     </row>
-    <row r="17" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="86"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="str">
@@ -4904,7 +4907,7 @@
       <c r="AL17" s="86"/>
       <c r="AM17" s="86"/>
     </row>
-    <row r="18" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="86"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="str">
@@ -4978,7 +4981,7 @@
       <c r="AL18" s="86"/>
       <c r="AM18" s="86"/>
     </row>
-    <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="86"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="str">
@@ -5052,7 +5055,7 @@
       <c r="AL19" s="86"/>
       <c r="AM19" s="86"/>
     </row>
-    <row r="20" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="86"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="str">
@@ -5126,7 +5129,7 @@
       <c r="AL20" s="86"/>
       <c r="AM20" s="86"/>
     </row>
-    <row r="21" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="86"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="str">
@@ -5200,7 +5203,7 @@
       <c r="AL21" s="86"/>
       <c r="AM21" s="86"/>
     </row>
-    <row r="22" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="86"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="str">
@@ -5274,7 +5277,7 @@
       <c r="AL22" s="86"/>
       <c r="AM22" s="86"/>
     </row>
-    <row r="23" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="86"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="str">
@@ -5338,7 +5341,7 @@
       <c r="AL23" s="86"/>
       <c r="AM23" s="86"/>
     </row>
-    <row r="24" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="86"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="str">
@@ -5369,7 +5372,7 @@
       <c r="AL24" s="86"/>
       <c r="AM24" s="86"/>
     </row>
-    <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="86"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="str">
@@ -5436,7 +5439,7 @@
       <c r="AL25" s="86"/>
       <c r="AM25" s="86"/>
     </row>
-    <row r="26" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="86"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="str">
@@ -5503,7 +5506,7 @@
       <c r="AL26" s="86"/>
       <c r="AM26" s="86"/>
     </row>
-    <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="86"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="str">
@@ -5578,7 +5581,7 @@
       <c r="AL27" s="86"/>
       <c r="AM27" s="86"/>
     </row>
-    <row r="28" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="86"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="str">
@@ -5653,7 +5656,7 @@
       <c r="AL28" s="86"/>
       <c r="AM28" s="86"/>
     </row>
-    <row r="29" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="86"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="str">
@@ -5728,7 +5731,7 @@
       <c r="AL29" s="86"/>
       <c r="AM29" s="86"/>
     </row>
-    <row r="30" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="86"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="str">
@@ -5803,7 +5806,7 @@
       <c r="AL30" s="86"/>
       <c r="AM30" s="86"/>
     </row>
-    <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="86"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="str">
@@ -5878,7 +5881,7 @@
       <c r="AL31" s="86"/>
       <c r="AM31" s="86"/>
     </row>
-    <row r="32" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="86"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="str">
@@ -5953,7 +5956,7 @@
       <c r="AL32" s="86"/>
       <c r="AM32" s="86"/>
     </row>
-    <row r="33" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="86"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="str">
@@ -6028,7 +6031,7 @@
       <c r="AL33" s="86"/>
       <c r="AM33" s="86"/>
     </row>
-    <row r="34" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="86"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="str">
@@ -6093,7 +6096,7 @@
       <c r="AL34" s="86"/>
       <c r="AM34" s="86"/>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A35" s="86"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="str">
@@ -6137,7 +6140,7 @@
       <c r="AL35" s="86"/>
       <c r="AM35" s="86"/>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A36" s="86"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="str">
@@ -6181,7 +6184,7 @@
       <c r="AL36" s="86"/>
       <c r="AM36" s="86"/>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A37" s="86"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="str">
@@ -6225,7 +6228,7 @@
       <c r="AL37" s="86"/>
       <c r="AM37" s="86"/>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A38" s="86"/>
       <c r="B38" s="86"/>
       <c r="C38" s="86"/>
@@ -6265,7 +6268,7 @@
       <c r="AK38" s="86"/>
       <c r="AL38" s="86"/>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A39" s="86"/>
       <c r="B39" s="86"/>
       <c r="C39" s="86"/>
@@ -6305,7 +6308,7 @@
       <c r="AK39" s="86"/>
       <c r="AL39" s="86"/>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A40" s="86"/>
       <c r="B40" s="86"/>
       <c r="C40" s="86"/>
@@ -6345,7 +6348,7 @@
       <c r="AK40" s="86"/>
       <c r="AL40" s="86"/>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A41" s="86"/>
       <c r="B41" s="86"/>
       <c r="C41" s="86"/>
@@ -6385,7 +6388,7 @@
       <c r="AK41" s="86"/>
       <c r="AL41" s="86"/>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A42" s="86"/>
       <c r="B42" s="86"/>
       <c r="C42" s="86"/>
@@ -6425,7 +6428,7 @@
       <c r="AK42" s="86"/>
       <c r="AL42" s="86"/>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A43" s="86"/>
       <c r="B43" s="86"/>
       <c r="C43" s="86"/>
@@ -6465,7 +6468,7 @@
       <c r="AK43" s="86"/>
       <c r="AL43" s="86"/>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A44" s="86"/>
       <c r="B44" s="86"/>
       <c r="C44" s="86"/>
@@ -6505,7 +6508,7 @@
       <c r="AK44" s="86"/>
       <c r="AL44" s="86"/>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A45" s="86"/>
       <c r="B45" s="86"/>
       <c r="C45" s="86"/>
@@ -6545,7 +6548,7 @@
       <c r="AK45" s="86"/>
       <c r="AL45" s="86"/>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A46" s="86"/>
       <c r="B46" s="86"/>
       <c r="C46" s="86"/>
@@ -6585,7 +6588,7 @@
       <c r="AK46" s="86"/>
       <c r="AL46" s="86"/>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A47" s="86"/>
       <c r="B47" s="86"/>
       <c r="C47" s="86"/>
@@ -6625,7 +6628,7 @@
       <c r="AK47" s="86"/>
       <c r="AL47" s="86"/>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A48" s="86"/>
       <c r="B48" s="86"/>
       <c r="C48" s="86"/>
@@ -6665,7 +6668,7 @@
       <c r="AK48" s="86"/>
       <c r="AL48" s="86"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A49" s="86"/>
       <c r="B49" s="86"/>
       <c r="C49" s="86"/>
@@ -6705,7 +6708,7 @@
       <c r="AK49" s="86"/>
       <c r="AL49" s="86"/>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A50" s="86"/>
       <c r="B50" s="86"/>
       <c r="C50" s="86"/>
@@ -6745,7 +6748,7 @@
       <c r="AK50" s="86"/>
       <c r="AL50" s="86"/>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A51" s="86"/>
       <c r="B51" s="86"/>
       <c r="C51" s="86"/>
@@ -6785,7 +6788,7 @@
       <c r="AK51" s="86"/>
       <c r="AL51" s="86"/>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A52" s="86"/>
       <c r="B52" s="86"/>
       <c r="C52" s="86"/>
@@ -6825,7 +6828,7 @@
       <c r="AK52" s="86"/>
       <c r="AL52" s="86"/>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A53" s="86"/>
       <c r="B53" s="86"/>
       <c r="C53" s="86"/>
@@ -6865,7 +6868,7 @@
       <c r="AK53" s="86"/>
       <c r="AL53" s="86"/>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A54" s="86"/>
       <c r="B54" s="86"/>
       <c r="C54" s="86"/>
@@ -6905,7 +6908,7 @@
       <c r="AK54" s="86"/>
       <c r="AL54" s="86"/>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A55" s="86"/>
       <c r="B55" s="86"/>
       <c r="C55" s="86"/>
@@ -6945,7 +6948,7 @@
       <c r="AK55" s="86"/>
       <c r="AL55" s="86"/>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A56" s="86"/>
       <c r="B56" s="86"/>
       <c r="C56" s="86"/>
@@ -6985,13 +6988,13 @@
       <c r="AK56" s="86"/>
       <c r="AL56" s="86"/>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A57" s="86"/>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A58" s="86"/>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A59" s="86"/>
     </row>
   </sheetData>
@@ -7191,47 +7194,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEF356-01A3-45DB-BFFF-83FE6984CD58}">
   <dimension ref="A1:AV182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AU8" sqref="AU8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="76.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="65.77734375" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="13" max="13" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5546875" customWidth="1"/>
-    <col min="17" max="17" width="73.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5546875" customWidth="1"/>
-    <col min="19" max="19" width="71.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5546875" customWidth="1"/>
-    <col min="21" max="21" width="61.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="61.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.21875" customWidth="1"/>
-    <col min="25" max="25" width="59.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.21875" customWidth="1"/>
+    <col min="1" max="2" width="76.36328125" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="65.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="13" max="13" width="70.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.54296875" customWidth="1"/>
+    <col min="17" max="17" width="73.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.54296875" customWidth="1"/>
+    <col min="19" max="19" width="71.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.54296875" customWidth="1"/>
+    <col min="21" max="21" width="61.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="61.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.1796875" customWidth="1"/>
+    <col min="25" max="25" width="59.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" customWidth="1"/>
     <col min="27" max="27" width="20" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="77.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="77.453125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="6" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="59" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="78.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.109375" customWidth="1"/>
-    <col min="46" max="46" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="78.5546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.08984375" customWidth="1"/>
+    <col min="46" max="46" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" ht="79.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="109" t="s">
         <v>74</v>
       </c>
@@ -7251,7 +7254,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -7376,7 +7379,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="str" cm="1">
         <f t="array" ref="A3">IFERROR(SUBSTITUTE(_xlfn._xlws.FILTER(_xlfn.UNIQUE(cha_mc[VisualId]&amp;cha_mc[TestName]),ISNUMBER(SEARCH(MC_Check!H2 &amp; "*LLC*__MCI_STATUS*", _xlfn.UNIQUE(cha_mc[VisualId]&amp;cha_mc[TestName])))),MC_Check!H2,""),"No LLC Data Found")</f>
         <v>No LLC Data Found</v>
@@ -7534,7 +7537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>130</v>
       </c>
@@ -7680,7 +7683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
       <c r="F5">
         <v>0</v>
       </c>
@@ -7823,7 +7826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
       <c r="F6">
         <v>0</v>
       </c>
@@ -7958,15 +7961,15 @@
         <v>118</v>
       </c>
       <c r="AU6" t="str">
-        <f>"*SOCKET0**COMPUTE0**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS"&amp;splitchar&amp;"MC*STATUS*"</f>
-        <v>*SOCKET0**COMPUTE0**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS__MC*STATUS*</v>
+        <f>"*SOCKET0**COMPUTE1**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS"&amp;splitchar&amp;"MC*STATUS*"</f>
+        <v>*SOCKET0**COMPUTE1**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS__MC*STATUS*</v>
       </c>
       <c r="AV6">
         <f>COUNTIFS(cha_mc[TestName],punitmcas[[#This Row],[MCA_String]],cha_mc[VisualId],MC_Check!$H$2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>132</v>
       </c>
@@ -8104,15 +8107,15 @@
         <v>119</v>
       </c>
       <c r="AU7" t="str">
-        <f>"*SOCKET0**COMPUTE0**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS"&amp;splitchar&amp;"MC*STATUS*"</f>
-        <v>*SOCKET0**COMPUTE0**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS__MC*STATUS*</v>
+        <f>"*SOCKET0**COMPUTE2**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS"&amp;splitchar&amp;"MC*STATUS*"</f>
+        <v>*SOCKET0**COMPUTE2**UNCORE**PUNIT**PTPCFSMS**PTPCFSMS__MC*STATUS*</v>
       </c>
       <c r="AV7">
         <f>COUNTIFS(cha_mc[TestName],punitmcas[[#This Row],[MCA_String]],cha_mc[VisualId],MC_Check!$H$2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D8">
         <v>1</v>
       </c>
@@ -8236,7 +8239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D9">
         <v>2</v>
       </c>
@@ -8361,7 +8364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D10">
         <v>3</v>
       </c>
@@ -8486,7 +8489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
       <c r="F11">
         <v>0</v>
       </c>
@@ -8608,7 +8611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.35">
       <c r="F12">
         <v>0</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>134</v>
       </c>
@@ -8853,7 +8856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>149</v>
       </c>
@@ -8977,7 +8980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>150</v>
       </c>
@@ -9085,7 +9088,7 @@
       <c r="AK15" s="65"/>
       <c r="AL15" s="65"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.35">
       <c r="F16">
         <v>0</v>
       </c>
@@ -9185,7 +9188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F17">
         <v>0</v>
       </c>
@@ -9197,7 +9200,7 @@
         <v>14</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="H17:I18" si="0">I10+1</f>
+        <f t="shared" ref="I17:I18" si="0">I10+1</f>
         <v>5</v>
       </c>
       <c r="J17" s="5" t="b">
@@ -9285,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F18">
         <v>0</v>
       </c>
@@ -9385,7 +9388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F19">
         <v>0</v>
       </c>
@@ -9484,7 +9487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F20">
         <v>0</v>
       </c>
@@ -9583,7 +9586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F21">
         <v>0</v>
       </c>
@@ -9682,7 +9685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F22">
         <v>0</v>
       </c>
@@ -9781,7 +9784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F23">
         <v>0</v>
       </c>
@@ -9881,7 +9884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F24">
         <v>0</v>
       </c>
@@ -9893,7 +9896,7 @@
         <v>21</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="H24:I25" si="1">I17+1</f>
+        <f t="shared" ref="I24:I25" si="1">I17+1</f>
         <v>6</v>
       </c>
       <c r="J24" s="5" t="b">
@@ -9981,7 +9984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F25">
         <v>0</v>
       </c>
@@ -10081,7 +10084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F26">
         <v>0</v>
       </c>
@@ -10180,7 +10183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F27">
         <v>0</v>
       </c>
@@ -10279,7 +10282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F28">
         <v>0</v>
       </c>
@@ -10378,7 +10381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F29">
         <v>0</v>
       </c>
@@ -10477,7 +10480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F30">
         <v>0</v>
       </c>
@@ -10577,7 +10580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F31">
         <v>0</v>
       </c>
@@ -10589,7 +10592,7 @@
         <v>28</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="H31:I32" si="2">I24+1</f>
+        <f t="shared" ref="I31:I32" si="2">I24+1</f>
         <v>7</v>
       </c>
       <c r="J31" s="5" t="b">
@@ -10677,7 +10680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F32">
         <v>0</v>
       </c>
@@ -10777,7 +10780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F33">
         <v>0</v>
       </c>
@@ -10876,7 +10879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F34">
         <v>0</v>
       </c>
@@ -10975,7 +10978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F35">
         <v>0</v>
       </c>
@@ -11074,7 +11077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F36">
         <v>0</v>
       </c>
@@ -11173,7 +11176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F37">
         <v>0</v>
       </c>
@@ -11273,7 +11276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F38">
         <v>0</v>
       </c>
@@ -11373,7 +11376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F39">
         <v>0</v>
       </c>
@@ -11473,7 +11476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F40">
         <v>0</v>
       </c>
@@ -11572,7 +11575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F41">
         <v>0</v>
       </c>
@@ -11671,7 +11674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F42">
         <v>0</v>
       </c>
@@ -11770,7 +11773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F43">
         <v>0</v>
       </c>
@@ -11869,7 +11872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F44">
         <v>0</v>
       </c>
@@ -11969,7 +11972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F45">
         <v>0</v>
       </c>
@@ -11981,7 +11984,7 @@
         <v>42</v>
       </c>
       <c r="I45">
-        <f t="shared" ref="H45:I46" si="3">I38+1</f>
+        <f t="shared" ref="I45:I46" si="3">I38+1</f>
         <v>17</v>
       </c>
       <c r="J45" s="5" t="b">
@@ -12069,7 +12072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F46">
         <v>0</v>
       </c>
@@ -12169,7 +12172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F47">
         <v>0</v>
       </c>
@@ -12268,7 +12271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F48">
         <v>0</v>
       </c>
@@ -12367,7 +12370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F49">
         <v>0</v>
       </c>
@@ -12466,7 +12469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F50">
         <v>0</v>
       </c>
@@ -12565,7 +12568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F51">
         <v>0</v>
       </c>
@@ -12665,7 +12668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F52">
         <v>0</v>
       </c>
@@ -12677,7 +12680,7 @@
         <v>49</v>
       </c>
       <c r="I52">
-        <f t="shared" ref="H52:I53" si="4">I45+1</f>
+        <f t="shared" ref="I52:I53" si="4">I45+1</f>
         <v>18</v>
       </c>
       <c r="J52" s="5" t="b">
@@ -12765,7 +12768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F53">
         <v>0</v>
       </c>
@@ -12865,7 +12868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F54">
         <v>0</v>
       </c>
@@ -12964,7 +12967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F55">
         <v>0</v>
       </c>
@@ -13063,7 +13066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F56">
         <v>0</v>
       </c>
@@ -13162,7 +13165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F57">
         <v>0</v>
       </c>
@@ -13261,7 +13264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F58">
         <v>0</v>
       </c>
@@ -13361,7 +13364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F59">
         <v>0</v>
       </c>
@@ -13373,7 +13376,7 @@
         <v>56</v>
       </c>
       <c r="I59">
-        <f t="shared" ref="H59:I60" si="5">I52+1</f>
+        <f t="shared" ref="I59:I60" si="5">I52+1</f>
         <v>19</v>
       </c>
       <c r="J59" s="5" t="b">
@@ -13461,7 +13464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F60">
         <v>0</v>
       </c>
@@ -13561,7 +13564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F61">
         <v>0</v>
       </c>
@@ -13660,7 +13663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F62">
         <v>0</v>
       </c>
@@ -13759,7 +13762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F63">
         <v>1</v>
       </c>
@@ -13859,7 +13862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F64">
         <v>1</v>
       </c>
@@ -13959,7 +13962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F65">
         <v>1</v>
       </c>
@@ -14059,7 +14062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F66">
         <v>1</v>
       </c>
@@ -14159,7 +14162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F67">
         <v>1</v>
       </c>
@@ -14259,7 +14262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F68">
         <v>1</v>
       </c>
@@ -14359,7 +14362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F69">
         <v>1</v>
       </c>
@@ -14460,7 +14463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F70">
         <v>1</v>
       </c>
@@ -14561,7 +14564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F71">
         <v>1</v>
       </c>
@@ -14662,7 +14665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F72">
         <v>1</v>
       </c>
@@ -14762,7 +14765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F73">
         <v>1</v>
       </c>
@@ -14862,7 +14865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F74">
         <v>1</v>
       </c>
@@ -14962,7 +14965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F75">
         <v>1</v>
       </c>
@@ -15062,7 +15065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F76">
         <v>1</v>
       </c>
@@ -15163,7 +15166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F77">
         <v>1</v>
       </c>
@@ -15176,7 +15179,7 @@
         <v>74</v>
       </c>
       <c r="I77">
-        <f t="shared" ref="H77:I78" si="7">I70+1</f>
+        <f t="shared" ref="I77:I78" si="7">I70+1</f>
         <v>29</v>
       </c>
       <c r="J77" s="5" t="b">
@@ -15264,7 +15267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F78">
         <v>1</v>
       </c>
@@ -15365,7 +15368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="79" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F79">
         <v>1</v>
       </c>
@@ -15465,7 +15468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F80">
         <v>1</v>
       </c>
@@ -15565,7 +15568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F81">
         <v>1</v>
       </c>
@@ -15665,7 +15668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F82">
         <v>1</v>
       </c>
@@ -15765,7 +15768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F83">
         <v>1</v>
       </c>
@@ -15866,7 +15869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F84">
         <v>1</v>
       </c>
@@ -15879,7 +15882,7 @@
         <v>81</v>
       </c>
       <c r="I84">
-        <f t="shared" ref="H84:I85" si="8">I77+1</f>
+        <f t="shared" ref="I84:I85" si="8">I77+1</f>
         <v>30</v>
       </c>
       <c r="J84" s="5" t="b">
@@ -15967,7 +15970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F85">
         <v>1</v>
       </c>
@@ -16068,7 +16071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F86">
         <v>1</v>
       </c>
@@ -16168,7 +16171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F87">
         <v>1</v>
       </c>
@@ -16268,7 +16271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F88">
         <v>1</v>
       </c>
@@ -16368,7 +16371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F89">
         <v>1</v>
       </c>
@@ -16468,7 +16471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F90">
         <v>1</v>
       </c>
@@ -16569,7 +16572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F91">
         <v>1</v>
       </c>
@@ -16582,7 +16585,7 @@
         <v>88</v>
       </c>
       <c r="I91">
-        <f t="shared" ref="H91:I92" si="9">I84+1</f>
+        <f t="shared" ref="I91:I92" si="9">I84+1</f>
         <v>31</v>
       </c>
       <c r="J91" s="5" t="b">
@@ -16670,7 +16673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F92">
         <v>1</v>
       </c>
@@ -16771,7 +16774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F93">
         <v>1</v>
       </c>
@@ -16871,7 +16874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F94">
         <v>1</v>
       </c>
@@ -16971,7 +16974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F95">
         <v>1</v>
       </c>
@@ -17071,7 +17074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F96">
         <v>1</v>
       </c>
@@ -17171,7 +17174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F97">
         <v>1</v>
       </c>
@@ -17272,7 +17275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F98">
         <v>1</v>
       </c>
@@ -17373,7 +17376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F99">
         <v>1</v>
       </c>
@@ -17474,7 +17477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F100">
         <v>1</v>
       </c>
@@ -17574,7 +17577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F101">
         <v>1</v>
       </c>
@@ -17674,7 +17677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F102">
         <v>1</v>
       </c>
@@ -17774,7 +17777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F103">
         <v>1</v>
       </c>
@@ -17874,7 +17877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F104">
         <v>1</v>
       </c>
@@ -17975,7 +17978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F105">
         <v>1</v>
       </c>
@@ -17988,7 +17991,7 @@
         <v>102</v>
       </c>
       <c r="I105">
-        <f t="shared" ref="H105:I106" si="11">I98+1</f>
+        <f t="shared" ref="I105:I106" si="11">I98+1</f>
         <v>41</v>
       </c>
       <c r="J105" s="5" t="b">
@@ -18076,7 +18079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F106">
         <v>1</v>
       </c>
@@ -18177,7 +18180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F107">
         <v>1</v>
       </c>
@@ -18277,7 +18280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="108" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F108">
         <v>1</v>
       </c>
@@ -18377,7 +18380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="109" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F109">
         <v>1</v>
       </c>
@@ -18477,7 +18480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="110" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F110">
         <v>1</v>
       </c>
@@ -18577,7 +18580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F111">
         <v>1</v>
       </c>
@@ -18678,7 +18681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F112">
         <v>1</v>
       </c>
@@ -18691,7 +18694,7 @@
         <v>109</v>
       </c>
       <c r="I112">
-        <f t="shared" ref="H112:I113" si="12">I105+1</f>
+        <f t="shared" ref="I112:I113" si="12">I105+1</f>
         <v>42</v>
       </c>
       <c r="J112" s="5" t="b">
@@ -18779,7 +18782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F113">
         <v>1</v>
       </c>
@@ -18880,7 +18883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F114">
         <v>1</v>
       </c>
@@ -18980,7 +18983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="115" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F115">
         <v>1</v>
       </c>
@@ -19080,7 +19083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="116" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F116">
         <v>1</v>
       </c>
@@ -19180,7 +19183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="117" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F117">
         <v>1</v>
       </c>
@@ -19280,7 +19283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="118" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F118">
         <v>1</v>
       </c>
@@ -19381,7 +19384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="119" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F119">
         <v>1</v>
       </c>
@@ -19394,7 +19397,7 @@
         <v>116</v>
       </c>
       <c r="I119">
-        <f t="shared" ref="H119:I120" si="13">I112+1</f>
+        <f t="shared" ref="I119:I120" si="13">I112+1</f>
         <v>43</v>
       </c>
       <c r="J119" s="5" t="b">
@@ -19482,7 +19485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="120" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F120">
         <v>1</v>
       </c>
@@ -19583,7 +19586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="121" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F121">
         <v>1</v>
       </c>
@@ -19683,7 +19686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="122" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F122">
         <v>1</v>
       </c>
@@ -19783,7 +19786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="123" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F123">
         <v>2</v>
       </c>
@@ -19883,7 +19886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="124" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F124">
         <v>2</v>
       </c>
@@ -19983,7 +19986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="125" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F125">
         <v>2</v>
       </c>
@@ -20083,7 +20086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="126" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F126">
         <v>2</v>
       </c>
@@ -20183,7 +20186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="127" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F127">
         <v>2</v>
       </c>
@@ -20283,7 +20286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="128" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F128">
         <v>2</v>
       </c>
@@ -20383,7 +20386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="129" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F129">
         <v>2</v>
       </c>
@@ -20484,7 +20487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="130" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F130">
         <v>2</v>
       </c>
@@ -20585,7 +20588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="131" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F131">
         <v>2</v>
       </c>
@@ -20686,7 +20689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="132" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F132">
         <v>2</v>
       </c>
@@ -20786,7 +20789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="133" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F133">
         <v>2</v>
       </c>
@@ -20886,7 +20889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="134" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F134">
         <v>2</v>
       </c>
@@ -20986,7 +20989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="135" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F135">
         <v>2</v>
       </c>
@@ -21086,7 +21089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="136" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F136">
         <v>2</v>
       </c>
@@ -21187,7 +21190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="137" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F137">
         <v>2</v>
       </c>
@@ -21200,7 +21203,7 @@
         <v>134</v>
       </c>
       <c r="I137">
-        <f t="shared" ref="H137:I138" si="15">I130+1</f>
+        <f t="shared" ref="I137:I138" si="15">I130+1</f>
         <v>53</v>
       </c>
       <c r="J137" s="5" t="b">
@@ -21288,7 +21291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="138" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F138">
         <v>2</v>
       </c>
@@ -21389,7 +21392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="139" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F139">
         <v>2</v>
       </c>
@@ -21489,7 +21492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="140" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F140">
         <v>2</v>
       </c>
@@ -21589,7 +21592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="141" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F141">
         <v>2</v>
       </c>
@@ -21689,7 +21692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="142" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F142">
         <v>2</v>
       </c>
@@ -21789,7 +21792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="143" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F143">
         <v>2</v>
       </c>
@@ -21890,7 +21893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="144" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F144">
         <v>2</v>
       </c>
@@ -21903,7 +21906,7 @@
         <v>141</v>
       </c>
       <c r="I144">
-        <f t="shared" ref="H144:I145" si="16">I137+1</f>
+        <f t="shared" ref="I144:I145" si="16">I137+1</f>
         <v>54</v>
       </c>
       <c r="J144" s="5" t="b">
@@ -21991,7 +21994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="145" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F145">
         <v>2</v>
       </c>
@@ -22092,7 +22095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="146" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F146">
         <v>2</v>
       </c>
@@ -22192,7 +22195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="147" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F147">
         <v>2</v>
       </c>
@@ -22292,7 +22295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="148" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F148">
         <v>2</v>
       </c>
@@ -22392,7 +22395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="149" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F149">
         <v>2</v>
       </c>
@@ -22492,7 +22495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="150" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F150">
         <v>2</v>
       </c>
@@ -22593,7 +22596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="151" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F151">
         <v>2</v>
       </c>
@@ -22606,7 +22609,7 @@
         <v>148</v>
       </c>
       <c r="I151">
-        <f t="shared" ref="H151:I152" si="17">I144+1</f>
+        <f t="shared" ref="I151:I152" si="17">I144+1</f>
         <v>55</v>
       </c>
       <c r="J151" s="5" t="b">
@@ -22694,7 +22697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="152" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F152">
         <v>2</v>
       </c>
@@ -22795,7 +22798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="153" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F153">
         <v>2</v>
       </c>
@@ -22895,7 +22898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="154" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F154">
         <v>2</v>
       </c>
@@ -22995,7 +22998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="155" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F155">
         <v>2</v>
       </c>
@@ -23095,7 +23098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="156" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F156">
         <v>2</v>
       </c>
@@ -23195,7 +23198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="157" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F157">
         <v>2</v>
       </c>
@@ -23296,7 +23299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="158" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F158">
         <v>2</v>
       </c>
@@ -23397,7 +23400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="159" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F159">
         <v>2</v>
       </c>
@@ -23498,7 +23501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="160" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F160">
         <v>2</v>
       </c>
@@ -23598,7 +23601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="161" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F161">
         <v>2</v>
       </c>
@@ -23698,7 +23701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="162" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F162">
         <v>2</v>
       </c>
@@ -23798,7 +23801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="163" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F163">
         <v>2</v>
       </c>
@@ -23898,7 +23901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="164" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F164">
         <v>2</v>
       </c>
@@ -23999,7 +24002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="165" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F165">
         <v>2</v>
       </c>
@@ -24012,7 +24015,7 @@
         <v>162</v>
       </c>
       <c r="I165">
-        <f t="shared" ref="H165:I166" si="19">I158+1</f>
+        <f t="shared" ref="I165:I166" si="19">I158+1</f>
         <v>65</v>
       </c>
       <c r="J165" s="5" t="b">
@@ -24100,7 +24103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="166" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F166">
         <v>2</v>
       </c>
@@ -24201,7 +24204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="167" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F167">
         <v>2</v>
       </c>
@@ -24301,7 +24304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="168" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F168">
         <v>2</v>
       </c>
@@ -24401,7 +24404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="169" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F169">
         <v>2</v>
       </c>
@@ -24501,7 +24504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="170" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F170">
         <v>2</v>
       </c>
@@ -24601,7 +24604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="171" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F171">
         <v>2</v>
       </c>
@@ -24702,7 +24705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="172" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F172">
         <v>2</v>
       </c>
@@ -24715,7 +24718,7 @@
         <v>169</v>
       </c>
       <c r="I172">
-        <f t="shared" ref="H172:I173" si="20">I165+1</f>
+        <f t="shared" ref="I172:I173" si="20">I165+1</f>
         <v>66</v>
       </c>
       <c r="J172" s="5" t="b">
@@ -24803,7 +24806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="173" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F173">
         <v>2</v>
       </c>
@@ -24904,7 +24907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="174" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F174">
         <v>2</v>
       </c>
@@ -25004,7 +25007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="175" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F175">
         <v>2</v>
       </c>
@@ -25104,7 +25107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="176" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F176">
         <v>2</v>
       </c>
@@ -25204,7 +25207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="177" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F177">
         <v>2</v>
       </c>
@@ -25304,7 +25307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="178" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F178">
         <v>2</v>
       </c>
@@ -25405,7 +25408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="179" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F179">
         <v>2</v>
       </c>
@@ -25418,7 +25421,7 @@
         <v>176</v>
       </c>
       <c r="I179">
-        <f t="shared" ref="H179:I180" si="21">I172+1</f>
+        <f t="shared" ref="I179:I180" si="21">I172+1</f>
         <v>67</v>
       </c>
       <c r="J179" s="5" t="b">
@@ -25506,7 +25509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="180" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F180">
         <v>2</v>
       </c>
@@ -25607,7 +25610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="181" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F181">
         <v>2</v>
       </c>
@@ -25707,7 +25710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="6:30" x14ac:dyDescent="0.3">
+    <row r="182" spans="6:30" x14ac:dyDescent="0.35">
       <c r="F182">
         <v>2</v>
       </c>

</xml_diff>